<commit_message>
Update Stoned Build Change Logs.xlsx
</commit_message>
<xml_diff>
--- a/Docs/Stoned Build Change Logs.xlsx
+++ b/Docs/Stoned Build Change Logs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shiel\Documents\Unity\Stoned_Unity\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81F4B4D2-9549-44A7-9FF6-D581484B48E8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{209E7912-71CF-4F4B-A387-022685D5D076}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="640" uniqueCount="540">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="653" uniqueCount="552">
   <si>
     <t>Stoned Builds Change Log</t>
   </si>
@@ -1645,6 +1645,42 @@
   </si>
   <si>
     <t>0_426</t>
+  </si>
+  <si>
+    <t>0_427</t>
+  </si>
+  <si>
+    <t>0_428</t>
+  </si>
+  <si>
+    <t>0_429</t>
+  </si>
+  <si>
+    <t>0_430</t>
+  </si>
+  <si>
+    <t>0_431</t>
+  </si>
+  <si>
+    <t>0_432</t>
+  </si>
+  <si>
+    <t>0_433</t>
+  </si>
+  <si>
+    <t>0_434</t>
+  </si>
+  <si>
+    <t>0_435</t>
+  </si>
+  <si>
+    <t>0_436</t>
+  </si>
+  <si>
+    <t>0_437</t>
+  </si>
+  <si>
+    <t>Added Force Launch ability</t>
   </si>
 </sst>
 </file>
@@ -2076,10 +2112,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E442"/>
+  <dimension ref="A1:E453"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A417" workbookViewId="0">
-      <selection activeCell="A440" sqref="A440:A442"/>
+    <sheetView tabSelected="1" topLeftCell="A423" workbookViewId="0">
+      <selection activeCell="E450" sqref="E450"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -5189,6 +5225,70 @@
     <row r="442" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A442" t="s">
         <v>539</v>
+      </c>
+    </row>
+    <row r="443" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A443" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="444" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A444" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="445" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A445" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="446" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A446" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="447" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A447" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="448" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A448" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="449" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A449" t="s">
+        <v>546</v>
+      </c>
+      <c r="B449" s="2">
+        <v>44143</v>
+      </c>
+      <c r="C449" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E449" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="450" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A450" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="451" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A451" t="s">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="452" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A452" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="453" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A453" t="s">
+        <v>550</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add cooldown to teleport ability
</commit_message>
<xml_diff>
--- a/Docs/Stoned Build Change Logs.xlsx
+++ b/Docs/Stoned Build Change Logs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shiel\Documents\Unity\Stoned_Unity\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2339FE0-D7DC-415C-8B61-BA30F7396A7D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A427E54-9849-4504-8DD9-1EE7870319D6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="656" uniqueCount="554">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="666" uniqueCount="561">
   <si>
     <t>Stoned Builds Change Log</t>
   </si>
@@ -1687,6 +1687,27 @@
   </si>
   <si>
     <t>Added Flashlight ability, Readded Touch controls</t>
+  </si>
+  <si>
+    <t>0_439</t>
+  </si>
+  <si>
+    <t>Added Crab and Cactus enemies</t>
+  </si>
+  <si>
+    <t>0_440</t>
+  </si>
+  <si>
+    <t>Added Cactus Round and Cactus Surface enemies</t>
+  </si>
+  <si>
+    <t>0_441</t>
+  </si>
+  <si>
+    <t>0_442</t>
+  </si>
+  <si>
+    <t>Add checkpoint pods, teleport cooldown</t>
   </si>
 </sst>
 </file>
@@ -2118,9 +2139,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E454"/>
+  <dimension ref="A1:E458"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A432" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A432" workbookViewId="0">
+      <selection activeCell="B459" sqref="B459"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
@@ -5307,6 +5330,53 @@
       </c>
       <c r="E454" t="s">
         <v>553</v>
+      </c>
+    </row>
+    <row r="455" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A455" t="s">
+        <v>554</v>
+      </c>
+      <c r="B455" s="2">
+        <v>44153</v>
+      </c>
+      <c r="C455" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E455" t="s">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="456" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A456" t="s">
+        <v>556</v>
+      </c>
+      <c r="B456" s="2">
+        <v>44154</v>
+      </c>
+      <c r="C456" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E456" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="457" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A457" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="458" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A458" t="s">
+        <v>559</v>
+      </c>
+      <c r="B458" s="2">
+        <v>44158</v>
+      </c>
+      <c r="C458" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E458" t="s">
+        <v>560</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update build number to 0.539
</commit_message>
<xml_diff>
--- a/Docs/Stoned Build Change Logs.xlsx
+++ b/Docs/Stoned Build Change Logs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shiel\Documents\Unity\Stoned_Unity\Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shiel\Documents\Unity\Stonicorn\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3180FB56-AEB0-4359-AC5C-7FBDAA733908}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18CEE2EE-A840-48B6-B225-F10D0FFF1C52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15" yWindow="0" windowWidth="13665" windowHeight="13080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="675" uniqueCount="568">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="767" uniqueCount="660">
   <si>
     <t>Stoned Builds Change Log</t>
   </si>
@@ -1729,6 +1729,282 @@
   </si>
   <si>
     <t>Extract managers out of GameManager</t>
+  </si>
+  <si>
+    <t>0_448</t>
+  </si>
+  <si>
+    <t>0_449</t>
+  </si>
+  <si>
+    <t>0_450</t>
+  </si>
+  <si>
+    <t>0_451</t>
+  </si>
+  <si>
+    <t>0_452</t>
+  </si>
+  <si>
+    <t>0_453</t>
+  </si>
+  <si>
+    <t>0_454</t>
+  </si>
+  <si>
+    <t>0_455</t>
+  </si>
+  <si>
+    <t>0_456</t>
+  </si>
+  <si>
+    <t>0_457</t>
+  </si>
+  <si>
+    <t>0_458</t>
+  </si>
+  <si>
+    <t>0_459</t>
+  </si>
+  <si>
+    <t>0_460</t>
+  </si>
+  <si>
+    <t>0_461</t>
+  </si>
+  <si>
+    <t>0_462</t>
+  </si>
+  <si>
+    <t>0_463</t>
+  </si>
+  <si>
+    <t>0_464</t>
+  </si>
+  <si>
+    <t>0_465</t>
+  </si>
+  <si>
+    <t>0_466</t>
+  </si>
+  <si>
+    <t>0_467</t>
+  </si>
+  <si>
+    <t>0_468</t>
+  </si>
+  <si>
+    <t>0_469</t>
+  </si>
+  <si>
+    <t>0_470</t>
+  </si>
+  <si>
+    <t>0_471</t>
+  </si>
+  <si>
+    <t>0_472</t>
+  </si>
+  <si>
+    <t>0_473</t>
+  </si>
+  <si>
+    <t>0_474</t>
+  </si>
+  <si>
+    <t>0_475</t>
+  </si>
+  <si>
+    <t>0_476</t>
+  </si>
+  <si>
+    <t>0_477</t>
+  </si>
+  <si>
+    <t>0_478</t>
+  </si>
+  <si>
+    <t>0_479</t>
+  </si>
+  <si>
+    <t>0_480</t>
+  </si>
+  <si>
+    <t>0_481</t>
+  </si>
+  <si>
+    <t>0_482</t>
+  </si>
+  <si>
+    <t>0_483</t>
+  </si>
+  <si>
+    <t>0_484</t>
+  </si>
+  <si>
+    <t>0_485</t>
+  </si>
+  <si>
+    <t>0_486</t>
+  </si>
+  <si>
+    <t>0_487</t>
+  </si>
+  <si>
+    <t>0_488</t>
+  </si>
+  <si>
+    <t>0_489</t>
+  </si>
+  <si>
+    <t>0_490</t>
+  </si>
+  <si>
+    <t>0_491</t>
+  </si>
+  <si>
+    <t>0_492</t>
+  </si>
+  <si>
+    <t>0_493</t>
+  </si>
+  <si>
+    <t>0_494</t>
+  </si>
+  <si>
+    <t>0_495</t>
+  </si>
+  <si>
+    <t>0_496</t>
+  </si>
+  <si>
+    <t>0_497</t>
+  </si>
+  <si>
+    <t>0_498</t>
+  </si>
+  <si>
+    <t>0_499</t>
+  </si>
+  <si>
+    <t>0_500</t>
+  </si>
+  <si>
+    <t>0_501</t>
+  </si>
+  <si>
+    <t>0_502</t>
+  </si>
+  <si>
+    <t>0_503</t>
+  </si>
+  <si>
+    <t>0_504</t>
+  </si>
+  <si>
+    <t>0_505</t>
+  </si>
+  <si>
+    <t>0_506</t>
+  </si>
+  <si>
+    <t>0_507</t>
+  </si>
+  <si>
+    <t>0_508</t>
+  </si>
+  <si>
+    <t>0_509</t>
+  </si>
+  <si>
+    <t>0_510</t>
+  </si>
+  <si>
+    <t>0_511</t>
+  </si>
+  <si>
+    <t>0_512</t>
+  </si>
+  <si>
+    <t>0_513</t>
+  </si>
+  <si>
+    <t>0_514</t>
+  </si>
+  <si>
+    <t>0_515</t>
+  </si>
+  <si>
+    <t>0_516</t>
+  </si>
+  <si>
+    <t>0_517</t>
+  </si>
+  <si>
+    <t>0_518</t>
+  </si>
+  <si>
+    <t>0_519</t>
+  </si>
+  <si>
+    <t>0_520</t>
+  </si>
+  <si>
+    <t>0_521</t>
+  </si>
+  <si>
+    <t>0_522</t>
+  </si>
+  <si>
+    <t>0_523</t>
+  </si>
+  <si>
+    <t>0_524</t>
+  </si>
+  <si>
+    <t>0_525</t>
+  </si>
+  <si>
+    <t>0_526</t>
+  </si>
+  <si>
+    <t>0_527</t>
+  </si>
+  <si>
+    <t>0_528</t>
+  </si>
+  <si>
+    <t>0_529</t>
+  </si>
+  <si>
+    <t>0_530</t>
+  </si>
+  <si>
+    <t>0_531</t>
+  </si>
+  <si>
+    <t>0_532</t>
+  </si>
+  <si>
+    <t>0_533</t>
+  </si>
+  <si>
+    <t>0_534</t>
+  </si>
+  <si>
+    <t>0_535</t>
+  </si>
+  <si>
+    <t>0_536</t>
+  </si>
+  <si>
+    <t>0_537</t>
+  </si>
+  <si>
+    <t>0_538</t>
+  </si>
+  <si>
+    <t>0_539</t>
   </si>
 </sst>
 </file>
@@ -1799,7 +2075,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -1808,10 +2084,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -2160,10 +2435,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E463"/>
+  <dimension ref="A1:E555"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A432" workbookViewId="0">
-      <selection activeCell="E464" sqref="E464"/>
+    <sheetView tabSelected="1" topLeftCell="A531" workbookViewId="0">
+      <selection activeCell="C555" sqref="C555"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2198,7 +2473,7 @@
       <c r="C5" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="1" t="s">
         <v>144</v>
       </c>
       <c r="E5" s="1" t="s">
@@ -2357,7 +2632,7 @@
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A17" s="6" t="s">
+      <c r="A17" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B17" s="2">
@@ -5441,6 +5716,469 @@
       </c>
       <c r="E463" t="s">
         <v>567</v>
+      </c>
+    </row>
+    <row r="464" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A464" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="465" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A465" t="s">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="466" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A466" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="467" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A467" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="468" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A468" t="s">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="469" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A469" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="470" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A470" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="471" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A471" t="s">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="472" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A472" t="s">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="473" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A473" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="474" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A474" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="475" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A475" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="476" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A476" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="477" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A477" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="478" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A478" t="s">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="479" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A479" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="480" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A480" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="481" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A481" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="482" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A482" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="483" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A483" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="484" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A484" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="485" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A485" t="s">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="486" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A486" t="s">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="487" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A487" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="488" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A488" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="489" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A489" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="490" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A490" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="491" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A491" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="492" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A492" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="493" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A493" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="494" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A494" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="495" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A495" t="s">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="496" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A496" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="497" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A497" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="498" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A498" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="499" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A499" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="500" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A500" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="501" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A501" t="s">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="502" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A502" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="503" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A503" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="504" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A504" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="505" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A505" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="506" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A506" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="507" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A507" t="s">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="508" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A508" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="509" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A509" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="510" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A510" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="511" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A511" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="512" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A512" t="s">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="513" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A513" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="514" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A514" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="515" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A515" t="s">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="516" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A516" t="s">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="517" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A517" t="s">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="518" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A518" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="519" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A519" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="520" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A520" t="s">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="521" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A521" t="s">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="522" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A522" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="523" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A523" t="s">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="524" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A524" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="525" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A525" t="s">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="526" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A526" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="527" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A527" t="s">
+        <v>631</v>
+      </c>
+    </row>
+    <row r="528" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A528" t="s">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="529" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A529" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="530" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A530" t="s">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="531" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A531" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="532" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A532" t="s">
+        <v>636</v>
+      </c>
+    </row>
+    <row r="533" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A533" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="534" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A534" t="s">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="535" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A535" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="536" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A536" t="s">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="537" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A537" t="s">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="538" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A538" t="s">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="539" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A539" t="s">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="540" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A540" t="s">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="541" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A541" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="542" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A542" t="s">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="543" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A543" t="s">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="544" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A544" t="s">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="545" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A545" t="s">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="546" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A546" t="s">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="547" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A547" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="548" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A548" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="549" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A549" t="s">
+        <v>653</v>
+      </c>
+    </row>
+    <row r="550" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A550" t="s">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="551" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A551" t="s">
+        <v>655</v>
+      </c>
+    </row>
+    <row r="552" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A552" t="s">
+        <v>656</v>
+      </c>
+    </row>
+    <row r="553" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A553" t="s">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="554" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A554" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="555" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A555" t="s">
+        <v>659</v>
+      </c>
+      <c r="B555" s="2">
+        <v>44806</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
copy Docs from Five-Part-Story
</commit_message>
<xml_diff>
--- a/Docs/Stoned Build Change Logs.xlsx
+++ b/Docs/Stoned Build Change Logs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shiel\Documents\Unity\Stoned_Unity\Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shiel\Documents\Unity\Stonicorn\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3180FB56-AEB0-4359-AC5C-7FBDAA733908}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{318D89C0-AC01-4E2D-8E9E-73B6F87543B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="675" uniqueCount="568">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="782" uniqueCount="670">
   <si>
     <t>Stoned Builds Change Log</t>
   </si>
@@ -1729,6 +1729,312 @@
   </si>
   <si>
     <t>Extract managers out of GameManager</t>
+  </si>
+  <si>
+    <t>0_448</t>
+  </si>
+  <si>
+    <t>0_449</t>
+  </si>
+  <si>
+    <t>0_450</t>
+  </si>
+  <si>
+    <t>0_451</t>
+  </si>
+  <si>
+    <t>0_452</t>
+  </si>
+  <si>
+    <t>0_453</t>
+  </si>
+  <si>
+    <t>0_454</t>
+  </si>
+  <si>
+    <t>0_455</t>
+  </si>
+  <si>
+    <t>0_456</t>
+  </si>
+  <si>
+    <t>0_457</t>
+  </si>
+  <si>
+    <t>0_458</t>
+  </si>
+  <si>
+    <t>0_459</t>
+  </si>
+  <si>
+    <t>0_460</t>
+  </si>
+  <si>
+    <t>0_461</t>
+  </si>
+  <si>
+    <t>0_462</t>
+  </si>
+  <si>
+    <t>0_463</t>
+  </si>
+  <si>
+    <t>0_464</t>
+  </si>
+  <si>
+    <t>0_465</t>
+  </si>
+  <si>
+    <t>0_466</t>
+  </si>
+  <si>
+    <t>0_467</t>
+  </si>
+  <si>
+    <t>0_468</t>
+  </si>
+  <si>
+    <t>0_469</t>
+  </si>
+  <si>
+    <t>0_470</t>
+  </si>
+  <si>
+    <t>0_471</t>
+  </si>
+  <si>
+    <t>0_472</t>
+  </si>
+  <si>
+    <t>0_473</t>
+  </si>
+  <si>
+    <t>0_474</t>
+  </si>
+  <si>
+    <t>0_475</t>
+  </si>
+  <si>
+    <t>0_476</t>
+  </si>
+  <si>
+    <t>0_477</t>
+  </si>
+  <si>
+    <t>0_478</t>
+  </si>
+  <si>
+    <t>0_479</t>
+  </si>
+  <si>
+    <t>0_480</t>
+  </si>
+  <si>
+    <t>0_481</t>
+  </si>
+  <si>
+    <t>0_482</t>
+  </si>
+  <si>
+    <t>0_483</t>
+  </si>
+  <si>
+    <t>0_484</t>
+  </si>
+  <si>
+    <t>0_485</t>
+  </si>
+  <si>
+    <t>0_486</t>
+  </si>
+  <si>
+    <t>0_487</t>
+  </si>
+  <si>
+    <t>0_488</t>
+  </si>
+  <si>
+    <t>0_489</t>
+  </si>
+  <si>
+    <t>0_490</t>
+  </si>
+  <si>
+    <t>0_491</t>
+  </si>
+  <si>
+    <t>0_492</t>
+  </si>
+  <si>
+    <t>0_493</t>
+  </si>
+  <si>
+    <t>0_494</t>
+  </si>
+  <si>
+    <t>0_495</t>
+  </si>
+  <si>
+    <t>0_496</t>
+  </si>
+  <si>
+    <t>0_497</t>
+  </si>
+  <si>
+    <t>0_498</t>
+  </si>
+  <si>
+    <t>0_499</t>
+  </si>
+  <si>
+    <t>0_500</t>
+  </si>
+  <si>
+    <t>0_501</t>
+  </si>
+  <si>
+    <t>0_502</t>
+  </si>
+  <si>
+    <t>0_503</t>
+  </si>
+  <si>
+    <t>0_504</t>
+  </si>
+  <si>
+    <t>0_505</t>
+  </si>
+  <si>
+    <t>0_506</t>
+  </si>
+  <si>
+    <t>0_507</t>
+  </si>
+  <si>
+    <t>0_508</t>
+  </si>
+  <si>
+    <t>0_509</t>
+  </si>
+  <si>
+    <t>0_510</t>
+  </si>
+  <si>
+    <t>0_511</t>
+  </si>
+  <si>
+    <t>0_512</t>
+  </si>
+  <si>
+    <t>0_513</t>
+  </si>
+  <si>
+    <t>0_514</t>
+  </si>
+  <si>
+    <t>0_515</t>
+  </si>
+  <si>
+    <t>0_516</t>
+  </si>
+  <si>
+    <t>0_517</t>
+  </si>
+  <si>
+    <t>0_518</t>
+  </si>
+  <si>
+    <t>0_519</t>
+  </si>
+  <si>
+    <t>0_520</t>
+  </si>
+  <si>
+    <t>0_521</t>
+  </si>
+  <si>
+    <t>0_522</t>
+  </si>
+  <si>
+    <t>0_523</t>
+  </si>
+  <si>
+    <t>0_524</t>
+  </si>
+  <si>
+    <t>0_525</t>
+  </si>
+  <si>
+    <t>0_526</t>
+  </si>
+  <si>
+    <t>0_527</t>
+  </si>
+  <si>
+    <t>0_528</t>
+  </si>
+  <si>
+    <t>0_529</t>
+  </si>
+  <si>
+    <t>0_530</t>
+  </si>
+  <si>
+    <t>0_531</t>
+  </si>
+  <si>
+    <t>0_532</t>
+  </si>
+  <si>
+    <t>0_533</t>
+  </si>
+  <si>
+    <t>0_534</t>
+  </si>
+  <si>
+    <t>0_535</t>
+  </si>
+  <si>
+    <t>0_536</t>
+  </si>
+  <si>
+    <t>0_537</t>
+  </si>
+  <si>
+    <t>0_538</t>
+  </si>
+  <si>
+    <t>0_539</t>
+  </si>
+  <si>
+    <t>Fixed some roadblock errors</t>
+  </si>
+  <si>
+    <t>0_540</t>
+  </si>
+  <si>
+    <t>Reduced size of planet</t>
+  </si>
+  <si>
+    <t>0_541</t>
+  </si>
+  <si>
+    <t>0_542</t>
+  </si>
+  <si>
+    <t>Removed Time Rewind ability, Pre-Rough draft of Forest cave level</t>
+  </si>
+  <si>
+    <t>0_543</t>
+  </si>
+  <si>
+    <t>Added blocking rock, Drafted Forest cave level</t>
+  </si>
+  <si>
+    <t>0_544</t>
+  </si>
+  <si>
+    <t>Drafted Forest cave level</t>
   </si>
 </sst>
 </file>
@@ -1799,7 +2105,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -1808,10 +2114,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -2160,10 +2465,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E463"/>
+  <dimension ref="A1:E560"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A432" workbookViewId="0">
-      <selection activeCell="E464" sqref="E464"/>
+    <sheetView tabSelected="1" topLeftCell="A544" workbookViewId="0">
+      <selection activeCell="A561" sqref="A561"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2198,7 +2503,7 @@
       <c r="C5" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="1" t="s">
         <v>144</v>
       </c>
       <c r="E5" s="1" t="s">
@@ -2357,7 +2662,7 @@
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A17" s="6" t="s">
+      <c r="A17" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B17" s="2">
@@ -5441,6 +5746,536 @@
       </c>
       <c r="E463" t="s">
         <v>567</v>
+      </c>
+    </row>
+    <row r="464" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A464" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="465" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A465" t="s">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="466" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A466" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="467" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A467" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="468" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A468" t="s">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="469" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A469" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="470" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A470" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="471" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A471" t="s">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="472" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A472" t="s">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="473" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A473" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="474" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A474" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="475" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A475" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="476" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A476" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="477" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A477" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="478" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A478" t="s">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="479" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A479" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="480" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A480" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="481" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A481" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="482" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A482" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="483" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A483" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="484" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A484" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="485" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A485" t="s">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="486" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A486" t="s">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="487" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A487" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="488" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A488" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="489" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A489" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="490" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A490" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="491" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A491" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="492" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A492" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="493" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A493" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="494" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A494" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="495" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A495" t="s">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="496" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A496" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="497" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A497" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="498" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A498" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="499" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A499" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="500" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A500" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="501" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A501" t="s">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="502" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A502" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="503" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A503" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="504" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A504" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="505" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A505" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="506" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A506" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="507" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A507" t="s">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="508" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A508" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="509" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A509" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="510" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A510" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="511" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A511" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="512" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A512" t="s">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="513" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A513" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="514" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A514" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="515" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A515" t="s">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="516" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A516" t="s">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="517" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A517" t="s">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="518" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A518" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="519" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A519" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="520" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A520" t="s">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="521" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A521" t="s">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="522" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A522" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="523" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A523" t="s">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="524" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A524" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="525" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A525" t="s">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="526" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A526" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="527" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A527" t="s">
+        <v>631</v>
+      </c>
+    </row>
+    <row r="528" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A528" t="s">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="529" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A529" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="530" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A530" t="s">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="531" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A531" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="532" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A532" t="s">
+        <v>636</v>
+      </c>
+    </row>
+    <row r="533" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A533" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="534" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A534" t="s">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="535" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A535" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="536" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A536" t="s">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="537" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A537" t="s">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="538" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A538" t="s">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="539" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A539" t="s">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="540" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A540" t="s">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="541" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A541" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="542" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A542" t="s">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="543" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A543" t="s">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="544" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A544" t="s">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="545" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A545" t="s">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="546" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A546" t="s">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="547" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A547" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="548" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A548" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="549" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A549" t="s">
+        <v>653</v>
+      </c>
+    </row>
+    <row r="550" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A550" t="s">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="551" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A551" t="s">
+        <v>655</v>
+      </c>
+    </row>
+    <row r="552" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A552" t="s">
+        <v>656</v>
+      </c>
+    </row>
+    <row r="553" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A553" t="s">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="554" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A554" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="555" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A555" t="s">
+        <v>659</v>
+      </c>
+      <c r="B555" s="2">
+        <v>44806</v>
+      </c>
+      <c r="C555" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E555" t="s">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="556" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A556" t="s">
+        <v>661</v>
+      </c>
+      <c r="B556" s="2">
+        <v>44809</v>
+      </c>
+      <c r="C556" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E556" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="557" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A557" t="s">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="558" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A558" t="s">
+        <v>664</v>
+      </c>
+      <c r="B558" s="2">
+        <v>44812</v>
+      </c>
+      <c r="C558" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E558" t="s">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="559" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A559" t="s">
+        <v>666</v>
+      </c>
+      <c r="B559" s="2">
+        <v>44814</v>
+      </c>
+      <c r="C559" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E559" t="s">
+        <v>667</v>
+      </c>
+    </row>
+    <row r="560" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A560" t="s">
+        <v>668</v>
+      </c>
+      <c r="B560" s="2">
+        <v>44825</v>
+      </c>
+      <c r="C560" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E560" t="s">
+        <v>669</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update Build Log for Build 551
</commit_message>
<xml_diff>
--- a/Docs/Stoned Build Change Logs.xlsx
+++ b/Docs/Stoned Build Change Logs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shiel\Documents\Unity\Stonicorn\Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shield\Documents\Unity\Stonicorn\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{318D89C0-AC01-4E2D-8E9E-73B6F87543B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F836C2D-A1B4-4C51-AC8D-1F6F25331DCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6090" yWindow="4050" windowWidth="19710" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="782" uniqueCount="670">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="794" uniqueCount="680">
   <si>
     <t>Stoned Builds Change Log</t>
   </si>
@@ -2035,6 +2035,36 @@
   </si>
   <si>
     <t>Drafted Forest cave level</t>
+  </si>
+  <si>
+    <t>0_545</t>
+  </si>
+  <si>
+    <t>0_546</t>
+  </si>
+  <si>
+    <t>0_547</t>
+  </si>
+  <si>
+    <t>0_548</t>
+  </si>
+  <si>
+    <t>0_549</t>
+  </si>
+  <si>
+    <t>0_550</t>
+  </si>
+  <si>
+    <t>0_551</t>
+  </si>
+  <si>
+    <t>First try for 2024 Version</t>
+  </si>
+  <si>
+    <t>Separate levels version</t>
+  </si>
+  <si>
+    <t>recorded 2024-07-07</t>
   </si>
 </sst>
 </file>
@@ -2465,35 +2495,37 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E560"/>
+  <dimension ref="A1:F567"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A544" workbookViewId="0">
-      <selection activeCell="A561" sqref="A561"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="5" topLeftCell="A543" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D567" sqref="D567"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="9.9296875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="3.796875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="11.265625" style="4" customWidth="1"/>
+    <col min="2" max="2" width="10.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="3.85546875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" style="4" customWidth="1"/>
+    <col min="5" max="5" width="24.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="5" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
@@ -2510,7 +2542,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -2524,7 +2556,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -2538,7 +2570,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -2552,7 +2584,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -2566,7 +2598,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -2580,7 +2612,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>33</v>
       </c>
@@ -2594,7 +2626,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>34</v>
       </c>
@@ -2608,7 +2640,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>9</v>
       </c>
@@ -2622,7 +2654,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>10</v>
       </c>
@@ -2636,7 +2668,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>11</v>
       </c>
@@ -2650,7 +2682,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>12</v>
       </c>
@@ -2661,7 +2693,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>13</v>
       </c>
@@ -2675,7 +2707,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>14</v>
       </c>
@@ -2689,7 +2721,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>15</v>
       </c>
@@ -2703,7 +2735,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>16</v>
       </c>
@@ -2717,7 +2749,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>43</v>
       </c>
@@ -2731,7 +2763,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>17</v>
       </c>
@@ -2745,7 +2777,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>18</v>
       </c>
@@ -2759,7 +2791,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>44</v>
       </c>
@@ -2770,7 +2802,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>19</v>
       </c>
@@ -2784,7 +2816,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>20</v>
       </c>
@@ -2798,7 +2830,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>21</v>
       </c>
@@ -2812,7 +2844,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>22</v>
       </c>
@@ -2826,7 +2858,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>23</v>
       </c>
@@ -2840,7 +2872,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>24</v>
       </c>
@@ -2854,7 +2886,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>45</v>
       </c>
@@ -2868,7 +2900,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>25</v>
       </c>
@@ -2882,7 +2914,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>61</v>
       </c>
@@ -2896,7 +2928,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>63</v>
       </c>
@@ -2910,7 +2942,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>64</v>
       </c>
@@ -2924,7 +2956,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>66</v>
       </c>
@@ -2938,7 +2970,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>68</v>
       </c>
@@ -2952,7 +2984,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>80</v>
       </c>
@@ -2966,7 +2998,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>78</v>
       </c>
@@ -2980,7 +3012,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>76</v>
       </c>
@@ -2994,7 +3026,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>75</v>
       </c>
@@ -3008,7 +3040,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>72</v>
       </c>
@@ -3022,7 +3054,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>70</v>
       </c>
@@ -3036,7 +3068,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>82</v>
       </c>
@@ -3050,7 +3082,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>84</v>
       </c>
@@ -3064,7 +3096,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>86</v>
       </c>
@@ -3078,7 +3110,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>88</v>
       </c>
@@ -3092,7 +3124,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>90</v>
       </c>
@@ -3106,7 +3138,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>94</v>
       </c>
@@ -3120,7 +3152,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>92</v>
       </c>
@@ -3134,7 +3166,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>96</v>
       </c>
@@ -3148,7 +3180,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>98</v>
       </c>
@@ -3162,7 +3194,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>101</v>
       </c>
@@ -3176,7 +3208,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>103</v>
       </c>
@@ -3190,7 +3222,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>105</v>
       </c>
@@ -3204,7 +3236,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>108</v>
       </c>
@@ -3218,7 +3250,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>110</v>
       </c>
@@ -3232,7 +3264,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>112</v>
       </c>
@@ -3246,137 +3278,137 @@
         <v>113</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>140</v>
       </c>
@@ -3390,7 +3422,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>142</v>
       </c>
@@ -3407,7 +3439,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>146</v>
       </c>
@@ -3424,7 +3456,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>149</v>
       </c>
@@ -3438,7 +3470,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>151</v>
       </c>
@@ -3455,7 +3487,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>154</v>
       </c>
@@ -3472,7 +3504,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>156</v>
       </c>
@@ -3486,7 +3518,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>158</v>
       </c>
@@ -3503,7 +3535,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>161</v>
       </c>
@@ -3520,7 +3552,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>163</v>
       </c>
@@ -3537,7 +3569,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>164</v>
       </c>
@@ -3554,7 +3586,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>168</v>
       </c>
@@ -3571,7 +3603,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>171</v>
       </c>
@@ -3588,7 +3620,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>173</v>
       </c>
@@ -3605,7 +3637,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>176</v>
       </c>
@@ -3622,7 +3654,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>179</v>
       </c>
@@ -3639,7 +3671,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>181</v>
       </c>
@@ -3656,7 +3688,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>184</v>
       </c>
@@ -3673,7 +3705,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>187</v>
       </c>
@@ -3690,7 +3722,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>189</v>
       </c>
@@ -3707,7 +3739,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>191</v>
       </c>
@@ -3724,162 +3756,162 @@
         <v>193</v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="130" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="131" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="132" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="132" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="133" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="133" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="134" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="134" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="135" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="135" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="136" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="136" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="137" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="137" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="138" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="138" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="139" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="139" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="140" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="140" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="141" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="141" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="142" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="142" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="143" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="143" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="144" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="144" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>225</v>
       </c>
@@ -3893,397 +3925,397 @@
         <v>226</v>
       </c>
     </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="161" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="161" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="162" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="162" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="163" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="163" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="164" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="164" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="165" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="165" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="166" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="166" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="167" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="167" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="168" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="168" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="169" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="169" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="170" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="170" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="171" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="171" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="172" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="172" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="173" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="173" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="174" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="174" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="175" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="175" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="176" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="176" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="177" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="177" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="178" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="178" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="179" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="179" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="180" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="180" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="181" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="181" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="182" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="182" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="183" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="183" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="184" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="184" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="185" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="185" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="186" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="186" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="187" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="187" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="188" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="188" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="189" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="189" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="190" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="190" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="191" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="191" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="192" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="192" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="193" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="193" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="194" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="194" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="195" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="195" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="196" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="196" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="197" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="197" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="198" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="198" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="199" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="199" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="200" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="200" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="201" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="201" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="202" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="202" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="203" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="203" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="204" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="204" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="205" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="205" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="206" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="206" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="207" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="207" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="208" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="208" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="209" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="209" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="210" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="210" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="211" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="211" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="212" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="212" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="213" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="213" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="214" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="214" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="215" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="215" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="216" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="216" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="217" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="217" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="218" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="218" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="219" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="219" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="220" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="220" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="221" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="221" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="222" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="222" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="223" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="223" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="224" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="224" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="225" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="225" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="226" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="226" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="227" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="227" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="228" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="228" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="229" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="229" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
         <v>297</v>
       </c>
     </row>
-    <row r="230" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="230" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="231" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="231" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="232" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="232" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="233" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="233" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="234" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="234" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="235" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="235" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="236" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="236" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="237" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="237" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
         <v>305</v>
       </c>
@@ -4297,17 +4329,17 @@
         <v>306</v>
       </c>
     </row>
-    <row r="238" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="238" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
         <v>307</v>
       </c>
     </row>
-    <row r="239" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="239" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="240" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="240" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
         <v>309</v>
       </c>
@@ -4321,17 +4353,17 @@
         <v>310</v>
       </c>
     </row>
-    <row r="241" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="241" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
         <v>311</v>
       </c>
     </row>
-    <row r="242" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="242" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="243" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="243" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
         <v>313</v>
       </c>
@@ -4348,27 +4380,27 @@
         <v>314</v>
       </c>
     </row>
-    <row r="244" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="244" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="245" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="245" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="246" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="246" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="247" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="247" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="248" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="248" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
         <v>319</v>
       </c>
@@ -4385,7 +4417,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="249" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="249" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
         <v>322</v>
       </c>
@@ -4396,7 +4428,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="250" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="250" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
         <v>323</v>
       </c>
@@ -4413,37 +4445,37 @@
         <v>324</v>
       </c>
     </row>
-    <row r="251" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="251" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="252" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="252" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="253" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="253" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
         <v>327</v>
       </c>
     </row>
-    <row r="254" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="254" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
         <v>328</v>
       </c>
     </row>
-    <row r="255" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="255" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="256" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="256" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="257" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="257" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
         <v>331</v>
       </c>
@@ -4460,7 +4492,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="258" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="258" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
         <v>333</v>
       </c>
@@ -4474,12 +4506,12 @@
         <v>334</v>
       </c>
     </row>
-    <row r="259" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="259" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
         <v>335</v>
       </c>
     </row>
-    <row r="260" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="260" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
         <v>336</v>
       </c>
@@ -4493,17 +4525,17 @@
         <v>337</v>
       </c>
     </row>
-    <row r="261" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="261" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="262" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="262" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="263" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="263" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
         <v>340</v>
       </c>
@@ -4517,47 +4549,47 @@
         <v>341</v>
       </c>
     </row>
-    <row r="264" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="264" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
         <v>342</v>
       </c>
     </row>
-    <row r="265" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="265" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
         <v>343</v>
       </c>
     </row>
-    <row r="266" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="266" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
         <v>344</v>
       </c>
     </row>
-    <row r="267" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="267" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
         <v>345</v>
       </c>
     </row>
-    <row r="268" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="268" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
         <v>346</v>
       </c>
     </row>
-    <row r="269" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="269" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
         <v>347</v>
       </c>
     </row>
-    <row r="270" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="270" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
         <v>348</v>
       </c>
     </row>
-    <row r="271" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="271" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
         <v>349</v>
       </c>
     </row>
-    <row r="272" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="272" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
         <v>350</v>
       </c>
@@ -4571,22 +4603,22 @@
         <v>351</v>
       </c>
     </row>
-    <row r="273" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="273" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
         <v>352</v>
       </c>
     </row>
-    <row r="274" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="274" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="275" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="275" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
         <v>354</v>
       </c>
     </row>
-    <row r="276" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="276" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
         <v>355</v>
       </c>
@@ -4600,77 +4632,77 @@
         <v>356</v>
       </c>
     </row>
-    <row r="277" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="277" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
         <v>357</v>
       </c>
     </row>
-    <row r="278" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="278" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A278" t="s">
         <v>358</v>
       </c>
     </row>
-    <row r="279" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="279" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A279" t="s">
         <v>359</v>
       </c>
     </row>
-    <row r="280" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="280" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A280" t="s">
         <v>360</v>
       </c>
     </row>
-    <row r="281" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="281" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A281" t="s">
         <v>361</v>
       </c>
     </row>
-    <row r="282" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="282" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A282" t="s">
         <v>362</v>
       </c>
     </row>
-    <row r="283" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="283" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A283" t="s">
         <v>363</v>
       </c>
     </row>
-    <row r="284" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="284" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
         <v>364</v>
       </c>
     </row>
-    <row r="285" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="285" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A285" t="s">
         <v>365</v>
       </c>
     </row>
-    <row r="286" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="286" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A286" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="287" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="287" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A287" t="s">
         <v>367</v>
       </c>
     </row>
-    <row r="288" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="288" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A288" t="s">
         <v>368</v>
       </c>
     </row>
-    <row r="289" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="289" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A289" t="s">
         <v>369</v>
       </c>
     </row>
-    <row r="290" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="290" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A290" t="s">
         <v>370</v>
       </c>
     </row>
-    <row r="291" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="291" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A291" t="s">
         <v>371</v>
       </c>
@@ -4684,132 +4716,132 @@
         <v>372</v>
       </c>
     </row>
-    <row r="292" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="292" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A292" t="s">
         <v>373</v>
       </c>
     </row>
-    <row r="293" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="293" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A293" t="s">
         <v>374</v>
       </c>
     </row>
-    <row r="294" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="294" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A294" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="295" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="295" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A295" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="296" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="296" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A296" t="s">
         <v>377</v>
       </c>
     </row>
-    <row r="297" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="297" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A297" t="s">
         <v>378</v>
       </c>
     </row>
-    <row r="298" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="298" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A298" t="s">
         <v>379</v>
       </c>
     </row>
-    <row r="299" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="299" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A299" t="s">
         <v>380</v>
       </c>
     </row>
-    <row r="300" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="300" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A300" t="s">
         <v>381</v>
       </c>
     </row>
-    <row r="301" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="301" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A301" t="s">
         <v>382</v>
       </c>
     </row>
-    <row r="302" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="302" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A302" t="s">
         <v>383</v>
       </c>
     </row>
-    <row r="303" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="303" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A303" t="s">
         <v>384</v>
       </c>
     </row>
-    <row r="304" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="304" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A304" t="s">
         <v>385</v>
       </c>
     </row>
-    <row r="305" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="305" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A305" t="s">
         <v>386</v>
       </c>
     </row>
-    <row r="306" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="306" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A306" t="s">
         <v>387</v>
       </c>
     </row>
-    <row r="307" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="307" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A307" t="s">
         <v>388</v>
       </c>
     </row>
-    <row r="308" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="308" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A308" t="s">
         <v>389</v>
       </c>
     </row>
-    <row r="309" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="309" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A309" t="s">
         <v>390</v>
       </c>
     </row>
-    <row r="310" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="310" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A310" t="s">
         <v>391</v>
       </c>
     </row>
-    <row r="311" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="311" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A311" t="s">
         <v>392</v>
       </c>
     </row>
-    <row r="312" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="312" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A312" t="s">
         <v>393</v>
       </c>
     </row>
-    <row r="313" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="313" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A313" t="s">
         <v>394</v>
       </c>
     </row>
-    <row r="314" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="314" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A314" t="s">
         <v>395</v>
       </c>
     </row>
-    <row r="315" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="315" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A315" t="s">
         <v>396</v>
       </c>
     </row>
-    <row r="316" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="316" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A316" t="s">
         <v>397</v>
       </c>
     </row>
-    <row r="317" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="317" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A317" t="s">
         <v>398</v>
       </c>
@@ -4823,62 +4855,62 @@
         <v>399</v>
       </c>
     </row>
-    <row r="318" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="318" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A318" t="s">
         <v>400</v>
       </c>
     </row>
-    <row r="319" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="319" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A319" t="s">
         <v>401</v>
       </c>
     </row>
-    <row r="320" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="320" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A320" t="s">
         <v>402</v>
       </c>
     </row>
-    <row r="321" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="321" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A321" t="s">
         <v>403</v>
       </c>
     </row>
-    <row r="322" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="322" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A322" t="s">
         <v>404</v>
       </c>
     </row>
-    <row r="323" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="323" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A323" t="s">
         <v>405</v>
       </c>
     </row>
-    <row r="324" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="324" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A324" t="s">
         <v>406</v>
       </c>
     </row>
-    <row r="325" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="325" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A325" t="s">
         <v>407</v>
       </c>
     </row>
-    <row r="326" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="326" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A326" t="s">
         <v>408</v>
       </c>
     </row>
-    <row r="327" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="327" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A327" t="s">
         <v>409</v>
       </c>
     </row>
-    <row r="328" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="328" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A328" t="s">
         <v>410</v>
       </c>
     </row>
-    <row r="329" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="329" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A329" t="s">
         <v>411</v>
       </c>
@@ -4895,7 +4927,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="330" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="330" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A330" t="s">
         <v>414</v>
       </c>
@@ -4912,47 +4944,47 @@
         <v>415</v>
       </c>
     </row>
-    <row r="331" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="331" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A331" t="s">
         <v>416</v>
       </c>
     </row>
-    <row r="332" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="332" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A332" t="s">
         <v>417</v>
       </c>
     </row>
-    <row r="333" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="333" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A333" t="s">
         <v>418</v>
       </c>
     </row>
-    <row r="334" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="334" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A334" t="s">
         <v>419</v>
       </c>
     </row>
-    <row r="335" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="335" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A335" t="s">
         <v>420</v>
       </c>
     </row>
-    <row r="336" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="336" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A336" t="s">
         <v>421</v>
       </c>
     </row>
-    <row r="337" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="337" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A337" t="s">
         <v>422</v>
       </c>
     </row>
-    <row r="338" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="338" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A338" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="339" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="339" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A339" t="s">
         <v>424</v>
       </c>
@@ -4966,182 +4998,182 @@
         <v>425</v>
       </c>
     </row>
-    <row r="340" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="340" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A340" t="s">
         <v>426</v>
       </c>
     </row>
-    <row r="341" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="341" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A341" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="342" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="342" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A342" t="s">
         <v>428</v>
       </c>
     </row>
-    <row r="343" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="343" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A343" t="s">
         <v>429</v>
       </c>
     </row>
-    <row r="344" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="344" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A344" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="345" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="345" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A345" t="s">
         <v>431</v>
       </c>
     </row>
-    <row r="346" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="346" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A346" t="s">
         <v>432</v>
       </c>
     </row>
-    <row r="347" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="347" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A347" t="s">
         <v>433</v>
       </c>
     </row>
-    <row r="348" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="348" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A348" t="s">
         <v>434</v>
       </c>
     </row>
-    <row r="349" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="349" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A349" t="s">
         <v>435</v>
       </c>
     </row>
-    <row r="350" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="350" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A350" t="s">
         <v>436</v>
       </c>
     </row>
-    <row r="351" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="351" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A351" t="s">
         <v>437</v>
       </c>
     </row>
-    <row r="352" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="352" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A352" t="s">
         <v>438</v>
       </c>
     </row>
-    <row r="353" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="353" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A353" t="s">
         <v>439</v>
       </c>
     </row>
-    <row r="354" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="354" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A354" t="s">
         <v>440</v>
       </c>
     </row>
-    <row r="355" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="355" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A355" t="s">
         <v>441</v>
       </c>
     </row>
-    <row r="356" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="356" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A356" t="s">
         <v>442</v>
       </c>
     </row>
-    <row r="357" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="357" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A357" t="s">
         <v>443</v>
       </c>
     </row>
-    <row r="358" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="358" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A358" t="s">
         <v>444</v>
       </c>
     </row>
-    <row r="359" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="359" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A359" t="s">
         <v>445</v>
       </c>
     </row>
-    <row r="360" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="360" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A360" t="s">
         <v>446</v>
       </c>
     </row>
-    <row r="361" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="361" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A361" t="s">
         <v>447</v>
       </c>
     </row>
-    <row r="362" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="362" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A362" t="s">
         <v>448</v>
       </c>
     </row>
-    <row r="363" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="363" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A363" t="s">
         <v>449</v>
       </c>
     </row>
-    <row r="364" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="364" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A364" t="s">
         <v>450</v>
       </c>
     </row>
-    <row r="365" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="365" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A365" t="s">
         <v>451</v>
       </c>
     </row>
-    <row r="366" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="366" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A366" t="s">
         <v>452</v>
       </c>
     </row>
-    <row r="367" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="367" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A367" t="s">
         <v>453</v>
       </c>
     </row>
-    <row r="368" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="368" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A368" t="s">
         <v>454</v>
       </c>
     </row>
-    <row r="369" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="369" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A369" t="s">
         <v>455</v>
       </c>
     </row>
-    <row r="370" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="370" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A370" t="s">
         <v>456</v>
       </c>
     </row>
-    <row r="371" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="371" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A371" t="s">
         <v>457</v>
       </c>
     </row>
-    <row r="372" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="372" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A372" t="s">
         <v>458</v>
       </c>
     </row>
-    <row r="373" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="373" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A373" t="s">
         <v>459</v>
       </c>
     </row>
-    <row r="374" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="374" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A374" t="s">
         <v>460</v>
       </c>
     </row>
-    <row r="375" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="375" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A375" t="s">
         <v>461</v>
       </c>
@@ -5155,57 +5187,57 @@
         <v>462</v>
       </c>
     </row>
-    <row r="376" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="376" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A376" t="s">
         <v>463</v>
       </c>
     </row>
-    <row r="377" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="377" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A377" t="s">
         <v>464</v>
       </c>
     </row>
-    <row r="378" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="378" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A378" t="s">
         <v>465</v>
       </c>
     </row>
-    <row r="379" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="379" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A379" t="s">
         <v>466</v>
       </c>
     </row>
-    <row r="380" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="380" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A380" t="s">
         <v>467</v>
       </c>
     </row>
-    <row r="381" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="381" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A381" t="s">
         <v>468</v>
       </c>
     </row>
-    <row r="382" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="382" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A382" t="s">
         <v>469</v>
       </c>
     </row>
-    <row r="383" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="383" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A383" t="s">
         <v>470</v>
       </c>
     </row>
-    <row r="384" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="384" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A384" t="s">
         <v>471</v>
       </c>
     </row>
-    <row r="385" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="385" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A385" t="s">
         <v>472</v>
       </c>
     </row>
-    <row r="386" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="386" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A386" t="s">
         <v>473</v>
       </c>
@@ -5219,52 +5251,52 @@
         <v>474</v>
       </c>
     </row>
-    <row r="387" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="387" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A387" t="s">
         <v>475</v>
       </c>
     </row>
-    <row r="388" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="388" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A388" t="s">
         <v>476</v>
       </c>
     </row>
-    <row r="389" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="389" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A389" t="s">
         <v>477</v>
       </c>
     </row>
-    <row r="390" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="390" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A390" t="s">
         <v>478</v>
       </c>
     </row>
-    <row r="391" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="391" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A391" t="s">
         <v>479</v>
       </c>
     </row>
-    <row r="392" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="392" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A392" t="s">
         <v>480</v>
       </c>
     </row>
-    <row r="393" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="393" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A393" t="s">
         <v>481</v>
       </c>
     </row>
-    <row r="394" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="394" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A394" t="s">
         <v>482</v>
       </c>
     </row>
-    <row r="395" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="395" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A395" t="s">
         <v>483</v>
       </c>
     </row>
-    <row r="396" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="396" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A396" t="s">
         <v>484</v>
       </c>
@@ -5278,62 +5310,62 @@
         <v>485</v>
       </c>
     </row>
-    <row r="397" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="397" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A397" t="s">
         <v>486</v>
       </c>
     </row>
-    <row r="398" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="398" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A398" t="s">
         <v>487</v>
       </c>
     </row>
-    <row r="399" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="399" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A399" t="s">
         <v>488</v>
       </c>
     </row>
-    <row r="400" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="400" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A400" t="s">
         <v>489</v>
       </c>
     </row>
-    <row r="401" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="401" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A401" t="s">
         <v>490</v>
       </c>
     </row>
-    <row r="402" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="402" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A402" t="s">
         <v>491</v>
       </c>
     </row>
-    <row r="403" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="403" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A403" t="s">
         <v>492</v>
       </c>
     </row>
-    <row r="404" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="404" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A404" t="s">
         <v>493</v>
       </c>
     </row>
-    <row r="405" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="405" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A405" t="s">
         <v>494</v>
       </c>
     </row>
-    <row r="406" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="406" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A406" t="s">
         <v>495</v>
       </c>
     </row>
-    <row r="407" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="407" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A407" t="s">
         <v>496</v>
       </c>
     </row>
-    <row r="408" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="408" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A408" t="s">
         <v>497</v>
       </c>
@@ -5347,7 +5379,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="409" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="409" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A409" t="s">
         <v>499</v>
       </c>
@@ -5361,22 +5393,22 @@
         <v>500</v>
       </c>
     </row>
-    <row r="410" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="410" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A410" t="s">
         <v>501</v>
       </c>
     </row>
-    <row r="411" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="411" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A411" t="s">
         <v>502</v>
       </c>
     </row>
-    <row r="412" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="412" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A412" t="s">
         <v>503</v>
       </c>
     </row>
-    <row r="413" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="413" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A413" t="s">
         <v>504</v>
       </c>
@@ -5390,17 +5422,17 @@
         <v>505</v>
       </c>
     </row>
-    <row r="414" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="414" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A414" t="s">
         <v>506</v>
       </c>
     </row>
-    <row r="415" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="415" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A415" t="s">
         <v>507</v>
       </c>
     </row>
-    <row r="416" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="416" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A416" t="s">
         <v>508</v>
       </c>
@@ -5414,17 +5446,17 @@
         <v>509</v>
       </c>
     </row>
-    <row r="417" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="417" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A417" t="s">
         <v>511</v>
       </c>
     </row>
-    <row r="418" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="418" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A418" t="s">
         <v>512</v>
       </c>
     </row>
-    <row r="419" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="419" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A419" t="s">
         <v>510</v>
       </c>
@@ -5438,42 +5470,42 @@
         <v>513</v>
       </c>
     </row>
-    <row r="420" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="420" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A420" t="s">
         <v>514</v>
       </c>
     </row>
-    <row r="421" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="421" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A421" t="s">
         <v>515</v>
       </c>
     </row>
-    <row r="422" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="422" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A422" t="s">
         <v>516</v>
       </c>
     </row>
-    <row r="423" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="423" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A423" t="s">
         <v>517</v>
       </c>
     </row>
-    <row r="424" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="424" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A424" t="s">
         <v>518</v>
       </c>
     </row>
-    <row r="425" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="425" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A425" t="s">
         <v>519</v>
       </c>
     </row>
-    <row r="426" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="426" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A426" t="s">
         <v>520</v>
       </c>
     </row>
-    <row r="427" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="427" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A427" t="s">
         <v>521</v>
       </c>
@@ -5487,47 +5519,47 @@
         <v>522</v>
       </c>
     </row>
-    <row r="428" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="428" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A428" t="s">
         <v>523</v>
       </c>
     </row>
-    <row r="429" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="429" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A429" t="s">
         <v>524</v>
       </c>
     </row>
-    <row r="430" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="430" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A430" t="s">
         <v>525</v>
       </c>
     </row>
-    <row r="431" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="431" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A431" t="s">
         <v>526</v>
       </c>
     </row>
-    <row r="432" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="432" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A432" t="s">
         <v>527</v>
       </c>
     </row>
-    <row r="433" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="433" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A433" t="s">
         <v>528</v>
       </c>
     </row>
-    <row r="434" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="434" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A434" t="s">
         <v>529</v>
       </c>
     </row>
-    <row r="435" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="435" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A435" t="s">
         <v>530</v>
       </c>
     </row>
-    <row r="436" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="436" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A436" t="s">
         <v>531</v>
       </c>
@@ -5541,27 +5573,27 @@
         <v>532</v>
       </c>
     </row>
-    <row r="437" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="437" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A437" t="s">
         <v>533</v>
       </c>
     </row>
-    <row r="438" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="438" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A438" t="s">
         <v>534</v>
       </c>
     </row>
-    <row r="439" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="439" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A439" t="s">
         <v>535</v>
       </c>
     </row>
-    <row r="440" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="440" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A440" t="s">
         <v>536</v>
       </c>
     </row>
-    <row r="441" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="441" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A441" t="s">
         <v>537</v>
       </c>
@@ -5575,42 +5607,42 @@
         <v>538</v>
       </c>
     </row>
-    <row r="442" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="442" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A442" t="s">
         <v>539</v>
       </c>
     </row>
-    <row r="443" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="443" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A443" t="s">
         <v>540</v>
       </c>
     </row>
-    <row r="444" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="444" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A444" t="s">
         <v>541</v>
       </c>
     </row>
-    <row r="445" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="445" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A445" t="s">
         <v>542</v>
       </c>
     </row>
-    <row r="446" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="446" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A446" t="s">
         <v>543</v>
       </c>
     </row>
-    <row r="447" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="447" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A447" t="s">
         <v>544</v>
       </c>
     </row>
-    <row r="448" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="448" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A448" t="s">
         <v>545</v>
       </c>
     </row>
-    <row r="449" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="449" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A449" t="s">
         <v>546</v>
       </c>
@@ -5624,27 +5656,27 @@
         <v>551</v>
       </c>
     </row>
-    <row r="450" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="450" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A450" t="s">
         <v>547</v>
       </c>
     </row>
-    <row r="451" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="451" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A451" t="s">
         <v>548</v>
       </c>
     </row>
-    <row r="452" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="452" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A452" t="s">
         <v>549</v>
       </c>
     </row>
-    <row r="453" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="453" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A453" t="s">
         <v>550</v>
       </c>
     </row>
-    <row r="454" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="454" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A454" t="s">
         <v>552</v>
       </c>
@@ -5658,7 +5690,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="455" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="455" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A455" t="s">
         <v>554</v>
       </c>
@@ -5672,7 +5704,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="456" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="456" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A456" t="s">
         <v>556</v>
       </c>
@@ -5686,12 +5718,12 @@
         <v>557</v>
       </c>
     </row>
-    <row r="457" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="457" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A457" t="s">
         <v>558</v>
       </c>
     </row>
-    <row r="458" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="458" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A458" t="s">
         <v>559</v>
       </c>
@@ -5705,12 +5737,12 @@
         <v>560</v>
       </c>
     </row>
-    <row r="459" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="459" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A459" t="s">
         <v>561</v>
       </c>
     </row>
-    <row r="460" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="460" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A460" t="s">
         <v>562</v>
       </c>
@@ -5724,17 +5756,17 @@
         <v>563</v>
       </c>
     </row>
-    <row r="461" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="461" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A461" t="s">
         <v>564</v>
       </c>
     </row>
-    <row r="462" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="462" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A462" t="s">
         <v>565</v>
       </c>
     </row>
-    <row r="463" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="463" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A463" t="s">
         <v>566</v>
       </c>
@@ -5748,462 +5780,474 @@
         <v>567</v>
       </c>
     </row>
-    <row r="464" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="464" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A464" t="s">
         <v>568</v>
       </c>
     </row>
-    <row r="465" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="465" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A465" t="s">
         <v>569</v>
       </c>
     </row>
-    <row r="466" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="466" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A466" t="s">
         <v>570</v>
       </c>
     </row>
-    <row r="467" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="467" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A467" t="s">
         <v>571</v>
       </c>
     </row>
-    <row r="468" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="468" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A468" t="s">
         <v>572</v>
       </c>
     </row>
-    <row r="469" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="469" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A469" t="s">
         <v>573</v>
       </c>
     </row>
-    <row r="470" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="470" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A470" t="s">
         <v>574</v>
       </c>
     </row>
-    <row r="471" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="471" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A471" t="s">
         <v>575</v>
       </c>
     </row>
-    <row r="472" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="472" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A472" t="s">
         <v>576</v>
       </c>
     </row>
-    <row r="473" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="473" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A473" t="s">
         <v>577</v>
       </c>
     </row>
-    <row r="474" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="474" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A474" t="s">
         <v>578</v>
       </c>
     </row>
-    <row r="475" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="475" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A475" t="s">
         <v>579</v>
       </c>
     </row>
-    <row r="476" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="476" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A476" t="s">
         <v>580</v>
       </c>
     </row>
-    <row r="477" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="477" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A477" t="s">
         <v>581</v>
       </c>
     </row>
-    <row r="478" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="478" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A478" t="s">
         <v>582</v>
       </c>
     </row>
-    <row r="479" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="479" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A479" t="s">
         <v>583</v>
       </c>
     </row>
-    <row r="480" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="480" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A480" t="s">
         <v>584</v>
       </c>
     </row>
-    <row r="481" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="481" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A481" t="s">
         <v>585</v>
       </c>
     </row>
-    <row r="482" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="482" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A482" t="s">
         <v>586</v>
       </c>
     </row>
-    <row r="483" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="483" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A483" t="s">
         <v>587</v>
       </c>
     </row>
-    <row r="484" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="484" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A484" t="s">
         <v>588</v>
       </c>
     </row>
-    <row r="485" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="485" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A485" t="s">
         <v>589</v>
       </c>
     </row>
-    <row r="486" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="486" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A486" t="s">
         <v>590</v>
       </c>
     </row>
-    <row r="487" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="487" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A487" t="s">
         <v>591</v>
       </c>
     </row>
-    <row r="488" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="488" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A488" t="s">
         <v>592</v>
       </c>
     </row>
-    <row r="489" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="489" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A489" t="s">
         <v>593</v>
       </c>
     </row>
-    <row r="490" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="490" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A490" t="s">
         <v>594</v>
       </c>
     </row>
-    <row r="491" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="491" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A491" t="s">
         <v>595</v>
       </c>
     </row>
-    <row r="492" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="492" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A492" t="s">
         <v>596</v>
       </c>
     </row>
-    <row r="493" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="493" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A493" t="s">
         <v>597</v>
       </c>
     </row>
-    <row r="494" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="494" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A494" t="s">
         <v>598</v>
       </c>
     </row>
-    <row r="495" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="495" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A495" t="s">
         <v>599</v>
       </c>
     </row>
-    <row r="496" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="496" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A496" t="s">
         <v>600</v>
       </c>
     </row>
-    <row r="497" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="497" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A497" t="s">
         <v>601</v>
       </c>
     </row>
-    <row r="498" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="498" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A498" t="s">
         <v>602</v>
       </c>
     </row>
-    <row r="499" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="499" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A499" t="s">
         <v>603</v>
       </c>
     </row>
-    <row r="500" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="500" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A500" t="s">
         <v>604</v>
       </c>
     </row>
-    <row r="501" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="501" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A501" t="s">
         <v>605</v>
       </c>
     </row>
-    <row r="502" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="502" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A502" t="s">
         <v>606</v>
       </c>
     </row>
-    <row r="503" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="503" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A503" t="s">
         <v>607</v>
       </c>
     </row>
-    <row r="504" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="504" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A504" t="s">
         <v>608</v>
       </c>
     </row>
-    <row r="505" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="505" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A505" t="s">
         <v>609</v>
       </c>
     </row>
-    <row r="506" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="506" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A506" t="s">
         <v>610</v>
       </c>
     </row>
-    <row r="507" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="507" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A507" t="s">
         <v>611</v>
       </c>
     </row>
-    <row r="508" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="508" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A508" t="s">
         <v>612</v>
       </c>
     </row>
-    <row r="509" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="509" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A509" t="s">
         <v>613</v>
       </c>
     </row>
-    <row r="510" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="510" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A510" t="s">
         <v>614</v>
       </c>
     </row>
-    <row r="511" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="511" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A511" t="s">
         <v>615</v>
       </c>
     </row>
-    <row r="512" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="512" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A512" t="s">
         <v>616</v>
       </c>
     </row>
-    <row r="513" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="513" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A513" t="s">
         <v>617</v>
       </c>
     </row>
-    <row r="514" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="514" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A514" t="s">
         <v>618</v>
       </c>
     </row>
-    <row r="515" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="515" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A515" t="s">
         <v>619</v>
       </c>
     </row>
-    <row r="516" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="516" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A516" t="s">
         <v>620</v>
       </c>
     </row>
-    <row r="517" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="517" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A517" t="s">
         <v>621</v>
       </c>
     </row>
-    <row r="518" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="518" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A518" t="s">
         <v>622</v>
       </c>
     </row>
-    <row r="519" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="519" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A519" t="s">
         <v>623</v>
       </c>
     </row>
-    <row r="520" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="520" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A520" t="s">
         <v>624</v>
       </c>
     </row>
-    <row r="521" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="521" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A521" t="s">
         <v>625</v>
       </c>
     </row>
-    <row r="522" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="522" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A522" t="s">
         <v>626</v>
       </c>
     </row>
-    <row r="523" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="523" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A523" t="s">
         <v>627</v>
       </c>
     </row>
-    <row r="524" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="524" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A524" t="s">
         <v>628</v>
       </c>
     </row>
-    <row r="525" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="525" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A525" t="s">
         <v>629</v>
       </c>
     </row>
-    <row r="526" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="526" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A526" t="s">
         <v>630</v>
       </c>
     </row>
-    <row r="527" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="527" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A527" t="s">
         <v>631</v>
       </c>
     </row>
-    <row r="528" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="528" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A528" t="s">
         <v>632</v>
       </c>
     </row>
-    <row r="529" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="529" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A529" t="s">
         <v>633</v>
       </c>
     </row>
-    <row r="530" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="530" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A530" t="s">
         <v>634</v>
       </c>
     </row>
-    <row r="531" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="531" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A531" t="s">
         <v>635</v>
       </c>
     </row>
-    <row r="532" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="532" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A532" t="s">
         <v>636</v>
       </c>
     </row>
-    <row r="533" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="533" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A533" t="s">
         <v>637</v>
       </c>
     </row>
-    <row r="534" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="534" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A534" t="s">
         <v>638</v>
       </c>
     </row>
-    <row r="535" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="535" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A535" t="s">
         <v>639</v>
       </c>
     </row>
-    <row r="536" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="536" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A536" t="s">
         <v>640</v>
       </c>
     </row>
-    <row r="537" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="537" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A537" t="s">
         <v>641</v>
       </c>
     </row>
-    <row r="538" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="538" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A538" t="s">
         <v>642</v>
       </c>
     </row>
-    <row r="539" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="539" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A539" t="s">
         <v>643</v>
       </c>
     </row>
-    <row r="540" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="540" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A540" t="s">
         <v>644</v>
       </c>
     </row>
-    <row r="541" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="541" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A541" t="s">
         <v>645</v>
       </c>
     </row>
-    <row r="542" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="542" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A542" t="s">
         <v>646</v>
       </c>
     </row>
-    <row r="543" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="543" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A543" t="s">
         <v>647</v>
       </c>
     </row>
-    <row r="544" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="544" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A544" t="s">
         <v>648</v>
       </c>
     </row>
-    <row r="545" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="545" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A545" t="s">
         <v>649</v>
       </c>
     </row>
-    <row r="546" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="546" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A546" t="s">
         <v>650</v>
       </c>
     </row>
-    <row r="547" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="547" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A547" t="s">
         <v>651</v>
       </c>
     </row>
-    <row r="548" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="548" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A548" t="s">
         <v>652</v>
       </c>
     </row>
-    <row r="549" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="549" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A549" t="s">
         <v>653</v>
       </c>
     </row>
-    <row r="550" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="550" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A550" t="s">
         <v>654</v>
       </c>
     </row>
-    <row r="551" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="551" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A551" t="s">
         <v>655</v>
       </c>
     </row>
-    <row r="552" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="552" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A552" t="s">
         <v>656</v>
       </c>
     </row>
-    <row r="553" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="553" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A553" t="s">
         <v>657</v>
       </c>
     </row>
-    <row r="554" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="554" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A554" t="s">
         <v>658</v>
       </c>
-    </row>
-    <row r="555" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B554" s="2">
+        <v>44509</v>
+      </c>
+      <c r="C554" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E554" t="s">
+        <v>678</v>
+      </c>
+      <c r="F554" t="s">
+        <v>679</v>
+      </c>
+    </row>
+    <row r="555" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A555" t="s">
         <v>659</v>
       </c>
@@ -6217,7 +6261,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="556" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="556" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A556" t="s">
         <v>661</v>
       </c>
@@ -6231,12 +6275,12 @@
         <v>662</v>
       </c>
     </row>
-    <row r="557" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="557" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A557" t="s">
         <v>663</v>
       </c>
     </row>
-    <row r="558" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="558" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A558" t="s">
         <v>664</v>
       </c>
@@ -6250,7 +6294,7 @@
         <v>665</v>
       </c>
     </row>
-    <row r="559" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="559" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A559" t="s">
         <v>666</v>
       </c>
@@ -6264,7 +6308,7 @@
         <v>667</v>
       </c>
     </row>
-    <row r="560" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="560" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A560" t="s">
         <v>668</v>
       </c>
@@ -6278,9 +6322,53 @@
         <v>669</v>
       </c>
     </row>
+    <row r="561" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A561" t="s">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="562" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A562" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="563" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A563" t="s">
+        <v>672</v>
+      </c>
+    </row>
+    <row r="564" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A564" t="s">
+        <v>673</v>
+      </c>
+    </row>
+    <row r="565" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A565" t="s">
+        <v>674</v>
+      </c>
+    </row>
+    <row r="566" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A566" t="s">
+        <v>675</v>
+      </c>
+    </row>
+    <row r="567" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A567" t="s">
+        <v>676</v>
+      </c>
+      <c r="B567" s="2">
+        <v>45480</v>
+      </c>
+      <c r="C567" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E567" t="s">
+        <v>677</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
-  <conditionalFormatting sqref="C1:D4 E95 E99 E102 C6:D1048576">
+  <conditionalFormatting sqref="C1:D4 C6:D1048576 E95 E99 E102">
     <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>"Unplayable"</formula>
     </cfRule>

</xml_diff>